<commit_message>
Update Tabella di  tracciabilità.xlsx
</commit_message>
<xml_diff>
--- a/Tabella di  tracciabilità.xlsx
+++ b/Tabella di  tracciabilità.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE46B72A-9B24-4286-BD64-A212D311CB3B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="1470" yWindow="1470" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="70">
   <si>
     <t>Requisiti</t>
   </si>
@@ -211,12 +212,30 @@
   </si>
   <si>
     <t>Mock-ups</t>
+  </si>
+  <si>
+    <t>Sottosistemi</t>
+  </si>
+  <si>
+    <t>Scontrino</t>
+  </si>
+  <si>
+    <t>Utenza</t>
+  </si>
+  <si>
+    <t>Ticket</t>
+  </si>
+  <si>
+    <t>Fornitura</t>
+  </si>
+  <si>
+    <t>Inventario</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
@@ -268,7 +287,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -291,6 +310,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -298,20 +348,11 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="2" applyBorder="1"/>
@@ -322,6 +363,22 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="20% - Colore 5" xfId="2" builtinId="46"/>
@@ -604,16 +661,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AP21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:BK21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" topLeftCell="AS1" workbookViewId="0">
+      <selection activeCell="BH11" sqref="BH11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:63" x14ac:dyDescent="0.25">
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -622,98 +679,121 @@
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
     </row>
-    <row r="2" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+    <row r="2" spans="1:63" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="6" t="s">
+      <c r="B2" s="8"/>
+      <c r="C2" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6" t="s">
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
-      <c r="N2" s="6"/>
-      <c r="O2" s="6"/>
-      <c r="P2" s="5" t="s">
+      <c r="K2" s="9"/>
+      <c r="L2" s="9"/>
+      <c r="M2" s="9"/>
+      <c r="N2" s="9"/>
+      <c r="O2" s="9"/>
+      <c r="P2" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="Q2" s="5"/>
-      <c r="R2" s="5"/>
-      <c r="S2" s="5"/>
-      <c r="T2" s="5"/>
-      <c r="U2" s="5"/>
-      <c r="V2" s="5" t="s">
+      <c r="Q2" s="8"/>
+      <c r="R2" s="8"/>
+      <c r="S2" s="8"/>
+      <c r="T2" s="8"/>
+      <c r="U2" s="8"/>
+      <c r="V2" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="W2" s="5"/>
-      <c r="X2" s="5"/>
-      <c r="Y2" s="5"/>
-      <c r="Z2" s="5"/>
-      <c r="AA2" s="5"/>
-      <c r="AB2" s="5" t="s">
+      <c r="W2" s="8"/>
+      <c r="X2" s="8"/>
+      <c r="Y2" s="8"/>
+      <c r="Z2" s="8"/>
+      <c r="AA2" s="8"/>
+      <c r="AB2" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="AC2" s="5"/>
-      <c r="AD2" s="5"/>
-      <c r="AE2" s="5"/>
-      <c r="AF2" s="5" t="s">
+      <c r="AC2" s="8"/>
+      <c r="AD2" s="8"/>
+      <c r="AE2" s="8"/>
+      <c r="AF2" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="AG2" s="5"/>
-      <c r="AH2" s="5"/>
-      <c r="AI2" s="5"/>
-      <c r="AJ2" s="5"/>
-      <c r="AK2" s="5"/>
-      <c r="AL2" s="5"/>
-      <c r="AM2" s="5"/>
-      <c r="AN2" s="5"/>
-      <c r="AO2" s="5"/>
-      <c r="AP2" s="5"/>
+      <c r="AG2" s="8"/>
+      <c r="AH2" s="8"/>
+      <c r="AI2" s="8"/>
+      <c r="AJ2" s="8"/>
+      <c r="AK2" s="8"/>
+      <c r="AL2" s="8"/>
+      <c r="AM2" s="8"/>
+      <c r="AN2" s="8"/>
+      <c r="AO2" s="8"/>
+      <c r="AP2" s="8"/>
+      <c r="AQ2" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="AR2" s="12"/>
+      <c r="AS2" s="12"/>
+      <c r="AT2" s="12"/>
+      <c r="AU2" s="12"/>
+      <c r="AV2" s="12"/>
+      <c r="AW2" s="12"/>
+      <c r="AX2" s="12"/>
+      <c r="AY2" s="12"/>
+      <c r="AZ2" s="12"/>
+      <c r="BA2" s="12"/>
+      <c r="BB2" s="12"/>
+      <c r="BC2" s="12"/>
+      <c r="BD2" s="12"/>
+      <c r="BE2" s="12"/>
+      <c r="BF2" s="12"/>
+      <c r="BG2" s="12"/>
+      <c r="BH2" s="12"/>
+      <c r="BI2" s="12"/>
+      <c r="BJ2" s="12"/>
+      <c r="BK2" s="13"/>
     </row>
-    <row r="3" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+    <row r="3" spans="1:63" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
       <c r="O3" s="2"/>
-      <c r="P3" s="7"/>
-      <c r="Q3" s="7"/>
-      <c r="R3" s="7"/>
-      <c r="S3" s="7"/>
-      <c r="T3" s="7"/>
-      <c r="U3" s="7"/>
+      <c r="P3" s="4"/>
+      <c r="Q3" s="4"/>
+      <c r="R3" s="4"/>
+      <c r="S3" s="4"/>
+      <c r="T3" s="4"/>
+      <c r="U3" s="4"/>
       <c r="V3" s="2"/>
       <c r="W3" s="2"/>
       <c r="X3" s="2"/>
       <c r="Y3" s="2"/>
       <c r="Z3" s="2"/>
       <c r="AA3" s="2"/>
-      <c r="AB3" s="9"/>
-      <c r="AC3" s="9"/>
-      <c r="AD3" s="9"/>
-      <c r="AE3" s="9"/>
+      <c r="AB3" s="6"/>
+      <c r="AC3" s="6"/>
+      <c r="AD3" s="6"/>
+      <c r="AE3" s="6"/>
       <c r="AF3" s="2"/>
       <c r="AG3" s="2"/>
       <c r="AH3" s="2"/>
@@ -727,41 +807,64 @@
       </c>
       <c r="AO3" s="2"/>
       <c r="AP3" s="2"/>
+      <c r="AQ3" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="AR3" s="2"/>
+      <c r="AS3" s="2"/>
+      <c r="AT3" s="2"/>
+      <c r="AU3" s="2"/>
+      <c r="AV3" s="2"/>
+      <c r="AW3" s="2"/>
+      <c r="AX3" s="2"/>
+      <c r="AY3" s="2"/>
+      <c r="AZ3" s="2"/>
+      <c r="BA3" s="2"/>
+      <c r="BB3" s="2"/>
+      <c r="BC3" s="2"/>
+      <c r="BD3" s="2"/>
+      <c r="BE3" s="2"/>
+      <c r="BF3" s="2"/>
+      <c r="BG3" s="2"/>
+      <c r="BH3" s="2"/>
+      <c r="BI3" s="2"/>
+      <c r="BJ3" s="2"/>
+      <c r="BK3" s="2"/>
     </row>
-    <row r="4" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+    <row r="4" spans="1:63" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
       <c r="O4" s="2"/>
-      <c r="P4" s="7"/>
-      <c r="Q4" s="7"/>
-      <c r="R4" s="7"/>
-      <c r="S4" s="7"/>
-      <c r="T4" s="7"/>
-      <c r="U4" s="7"/>
+      <c r="P4" s="4"/>
+      <c r="Q4" s="4"/>
+      <c r="R4" s="4"/>
+      <c r="S4" s="4"/>
+      <c r="T4" s="4"/>
+      <c r="U4" s="4"/>
       <c r="V4" s="2"/>
       <c r="W4" s="2"/>
       <c r="X4" s="2"/>
       <c r="Y4" s="2"/>
       <c r="Z4" s="2"/>
       <c r="AA4" s="2"/>
-      <c r="AB4" s="9"/>
-      <c r="AC4" s="9"/>
-      <c r="AD4" s="9"/>
-      <c r="AE4" s="9"/>
+      <c r="AB4" s="6"/>
+      <c r="AC4" s="6"/>
+      <c r="AD4" s="6"/>
+      <c r="AE4" s="6"/>
       <c r="AF4" s="2"/>
       <c r="AG4" s="2"/>
       <c r="AH4" s="2"/>
@@ -773,21 +876,42 @@
       <c r="AN4" s="2"/>
       <c r="AO4" s="2"/>
       <c r="AP4" s="2"/>
+      <c r="AQ4" s="2"/>
+      <c r="AR4" s="2"/>
+      <c r="AS4" s="2"/>
+      <c r="AT4" s="2"/>
+      <c r="AU4" s="2"/>
+      <c r="AV4" s="2"/>
+      <c r="AW4" s="2"/>
+      <c r="AX4" s="2"/>
+      <c r="AY4" s="2"/>
+      <c r="AZ4" s="2"/>
+      <c r="BA4" s="2"/>
+      <c r="BB4" s="2"/>
+      <c r="BC4" s="2"/>
+      <c r="BD4" s="2"/>
+      <c r="BE4" s="2"/>
+      <c r="BF4" s="2"/>
+      <c r="BG4" s="2"/>
+      <c r="BH4" s="2"/>
+      <c r="BI4" s="2"/>
+      <c r="BJ4" s="2"/>
+      <c r="BK4" s="2"/>
     </row>
-    <row r="5" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+    <row r="5" spans="1:63" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="8" t="s">
+      <c r="B5" s="10"/>
+      <c r="C5" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
       <c r="J5" s="3" t="s">
         <v>29</v>
       </c>
@@ -796,14 +920,14 @@
       <c r="M5" s="3"/>
       <c r="N5" s="3"/>
       <c r="O5" s="3"/>
-      <c r="P5" s="8" t="s">
+      <c r="P5" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="Q5" s="7"/>
-      <c r="R5" s="8"/>
-      <c r="S5" s="7"/>
-      <c r="T5" s="7"/>
-      <c r="U5" s="7"/>
+      <c r="Q5" s="4"/>
+      <c r="R5" s="5"/>
+      <c r="S5" s="4"/>
+      <c r="T5" s="4"/>
+      <c r="U5" s="4"/>
       <c r="V5" s="3" t="s">
         <v>43</v>
       </c>
@@ -812,12 +936,12 @@
       <c r="Y5" s="3"/>
       <c r="Z5" s="3"/>
       <c r="AA5" s="3"/>
-      <c r="AB5" s="10" t="s">
+      <c r="AB5" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="AC5" s="10"/>
-      <c r="AD5" s="9"/>
-      <c r="AE5" s="9"/>
+      <c r="AC5" s="7"/>
+      <c r="AD5" s="6"/>
+      <c r="AE5" s="6"/>
       <c r="AF5" s="2"/>
       <c r="AG5" s="2"/>
       <c r="AH5" s="2"/>
@@ -831,41 +955,64 @@
       <c r="AP5" s="2" t="s">
         <v>62</v>
       </c>
+      <c r="AQ5" s="2"/>
+      <c r="AR5" s="2"/>
+      <c r="AS5" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="AT5" s="2"/>
+      <c r="AU5" s="2"/>
+      <c r="AV5" s="2"/>
+      <c r="AW5" s="2"/>
+      <c r="AX5" s="2"/>
+      <c r="AY5" s="2"/>
+      <c r="AZ5" s="2"/>
+      <c r="BA5" s="2"/>
+      <c r="BB5" s="2"/>
+      <c r="BC5" s="2"/>
+      <c r="BD5" s="2"/>
+      <c r="BE5" s="2"/>
+      <c r="BF5" s="2"/>
+      <c r="BG5" s="2"/>
+      <c r="BH5" s="2"/>
+      <c r="BI5" s="2"/>
+      <c r="BJ5" s="2"/>
+      <c r="BK5" s="2"/>
     </row>
-    <row r="6" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+    <row r="6" spans="1:63" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
       <c r="M6" s="3"/>
       <c r="N6" s="3"/>
       <c r="O6" s="3"/>
-      <c r="P6" s="8"/>
-      <c r="Q6" s="7"/>
-      <c r="R6" s="8"/>
-      <c r="S6" s="7"/>
-      <c r="T6" s="7"/>
-      <c r="U6" s="7"/>
+      <c r="P6" s="5"/>
+      <c r="Q6" s="4"/>
+      <c r="R6" s="5"/>
+      <c r="S6" s="4"/>
+      <c r="T6" s="4"/>
+      <c r="U6" s="4"/>
       <c r="V6" s="3"/>
       <c r="W6" s="3"/>
       <c r="X6" s="3"/>
       <c r="Y6" s="3"/>
       <c r="Z6" s="3"/>
       <c r="AA6" s="3"/>
-      <c r="AB6" s="9"/>
-      <c r="AC6" s="9"/>
-      <c r="AD6" s="9"/>
-      <c r="AE6" s="9"/>
+      <c r="AB6" s="6"/>
+      <c r="AC6" s="6"/>
+      <c r="AD6" s="6"/>
+      <c r="AE6" s="6"/>
       <c r="AF6" s="2"/>
       <c r="AG6" s="2"/>
       <c r="AH6" s="2"/>
@@ -879,41 +1026,62 @@
       <c r="AN6" s="2"/>
       <c r="AO6" s="2"/>
       <c r="AP6" s="2"/>
+      <c r="AQ6" s="2"/>
+      <c r="AR6" s="2"/>
+      <c r="AS6" s="2"/>
+      <c r="AT6" s="2"/>
+      <c r="AU6" s="2"/>
+      <c r="AV6" s="2"/>
+      <c r="AW6" s="2"/>
+      <c r="AX6" s="2"/>
+      <c r="AY6" s="2"/>
+      <c r="AZ6" s="2"/>
+      <c r="BA6" s="2"/>
+      <c r="BB6" s="2"/>
+      <c r="BC6" s="2"/>
+      <c r="BD6" s="2"/>
+      <c r="BE6" s="2"/>
+      <c r="BF6" s="2"/>
+      <c r="BG6" s="2"/>
+      <c r="BH6" s="2"/>
+      <c r="BI6" s="2"/>
+      <c r="BJ6" s="2"/>
+      <c r="BK6" s="2"/>
     </row>
-    <row r="7" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+    <row r="7" spans="1:63" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
       <c r="M7" s="3"/>
       <c r="N7" s="3"/>
       <c r="O7" s="3"/>
-      <c r="P7" s="8"/>
-      <c r="Q7" s="7"/>
-      <c r="R7" s="8"/>
-      <c r="S7" s="7"/>
-      <c r="T7" s="7"/>
-      <c r="U7" s="7"/>
+      <c r="P7" s="5"/>
+      <c r="Q7" s="4"/>
+      <c r="R7" s="5"/>
+      <c r="S7" s="4"/>
+      <c r="T7" s="4"/>
+      <c r="U7" s="4"/>
       <c r="V7" s="3"/>
       <c r="W7" s="3"/>
       <c r="X7" s="3"/>
       <c r="Y7" s="3"/>
       <c r="Z7" s="3"/>
       <c r="AA7" s="3"/>
-      <c r="AB7" s="9"/>
-      <c r="AC7" s="9"/>
-      <c r="AD7" s="9"/>
-      <c r="AE7" s="9"/>
+      <c r="AB7" s="6"/>
+      <c r="AC7" s="6"/>
+      <c r="AD7" s="6"/>
+      <c r="AE7" s="6"/>
       <c r="AF7" s="2"/>
       <c r="AG7" s="2"/>
       <c r="AH7" s="2"/>
@@ -927,41 +1095,64 @@
         <v>61</v>
       </c>
       <c r="AP7" s="2"/>
+      <c r="AQ7" s="2"/>
+      <c r="AR7" s="2"/>
+      <c r="AS7" s="2"/>
+      <c r="AT7" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="AU7" s="2"/>
+      <c r="AV7" s="2"/>
+      <c r="AW7" s="2"/>
+      <c r="AX7" s="2"/>
+      <c r="AY7" s="2"/>
+      <c r="AZ7" s="2"/>
+      <c r="BA7" s="2"/>
+      <c r="BB7" s="2"/>
+      <c r="BC7" s="2"/>
+      <c r="BD7" s="2"/>
+      <c r="BE7" s="2"/>
+      <c r="BF7" s="2"/>
+      <c r="BG7" s="2"/>
+      <c r="BH7" s="2"/>
+      <c r="BI7" s="2"/>
+      <c r="BJ7" s="2"/>
+      <c r="BK7" s="2"/>
     </row>
-    <row r="8" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+    <row r="8" spans="1:63" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="4"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
       <c r="M8" s="3"/>
       <c r="N8" s="3"/>
       <c r="O8" s="3"/>
-      <c r="P8" s="8"/>
-      <c r="Q8" s="7"/>
-      <c r="R8" s="8"/>
-      <c r="S8" s="7"/>
-      <c r="T8" s="7"/>
-      <c r="U8" s="7"/>
+      <c r="P8" s="5"/>
+      <c r="Q8" s="4"/>
+      <c r="R8" s="5"/>
+      <c r="S8" s="4"/>
+      <c r="T8" s="4"/>
+      <c r="U8" s="4"/>
       <c r="V8" s="3"/>
       <c r="W8" s="3"/>
       <c r="X8" s="3"/>
       <c r="Y8" s="3"/>
       <c r="Z8" s="3"/>
       <c r="AA8" s="3"/>
-      <c r="AB8" s="9"/>
-      <c r="AC8" s="9"/>
-      <c r="AD8" s="9"/>
-      <c r="AE8" s="9"/>
+      <c r="AB8" s="6"/>
+      <c r="AC8" s="6"/>
+      <c r="AD8" s="6"/>
+      <c r="AE8" s="6"/>
       <c r="AF8" s="2"/>
       <c r="AG8" s="2"/>
       <c r="AH8" s="2"/>
@@ -973,43 +1164,66 @@
       <c r="AN8" s="2"/>
       <c r="AO8" s="2"/>
       <c r="AP8" s="2"/>
+      <c r="AQ8" s="2"/>
+      <c r="AR8" s="2"/>
+      <c r="AS8" s="2"/>
+      <c r="AT8" s="2"/>
+      <c r="AU8" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="AV8" s="2"/>
+      <c r="AW8" s="2"/>
+      <c r="AX8" s="2"/>
+      <c r="AY8" s="2"/>
+      <c r="AZ8" s="2"/>
+      <c r="BA8" s="2"/>
+      <c r="BB8" s="2"/>
+      <c r="BC8" s="2"/>
+      <c r="BD8" s="2"/>
+      <c r="BE8" s="2"/>
+      <c r="BF8" s="2"/>
+      <c r="BG8" s="2"/>
+      <c r="BH8" s="2"/>
+      <c r="BI8" s="2"/>
+      <c r="BJ8" s="2"/>
+      <c r="BK8" s="2"/>
     </row>
-    <row r="9" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+    <row r="9" spans="1:63" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="4"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="8" t="s">
+      <c r="B9" s="10"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
       <c r="M9" s="3"/>
       <c r="N9" s="3"/>
       <c r="O9" s="3"/>
-      <c r="P9" s="8"/>
-      <c r="Q9" s="7"/>
-      <c r="R9" s="8"/>
-      <c r="S9" s="7"/>
-      <c r="T9" s="7"/>
-      <c r="U9" s="7"/>
+      <c r="P9" s="5"/>
+      <c r="Q9" s="4"/>
+      <c r="R9" s="5"/>
+      <c r="S9" s="4"/>
+      <c r="T9" s="4"/>
+      <c r="U9" s="4"/>
       <c r="V9" s="3"/>
       <c r="W9" s="3"/>
       <c r="X9" s="3"/>
       <c r="Y9" s="3"/>
       <c r="Z9" s="3"/>
       <c r="AA9" s="3"/>
-      <c r="AB9" s="9"/>
-      <c r="AC9" s="9"/>
-      <c r="AD9" s="9"/>
-      <c r="AE9" s="9"/>
+      <c r="AB9" s="6"/>
+      <c r="AC9" s="6"/>
+      <c r="AD9" s="6"/>
+      <c r="AE9" s="6"/>
       <c r="AF9" s="2" t="s">
         <v>52</v>
       </c>
@@ -1023,41 +1237,64 @@
       <c r="AN9" s="2"/>
       <c r="AO9" s="2"/>
       <c r="AP9" s="2"/>
+      <c r="AQ9" s="2"/>
+      <c r="AR9" s="2"/>
+      <c r="AS9" s="2"/>
+      <c r="AT9" s="2"/>
+      <c r="AU9" s="2"/>
+      <c r="AV9" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="AW9" s="2"/>
+      <c r="AX9" s="2"/>
+      <c r="AY9" s="2"/>
+      <c r="AZ9" s="2"/>
+      <c r="BA9" s="2"/>
+      <c r="BB9" s="2"/>
+      <c r="BC9" s="2"/>
+      <c r="BD9" s="2"/>
+      <c r="BE9" s="2"/>
+      <c r="BF9" s="2"/>
+      <c r="BG9" s="2"/>
+      <c r="BH9" s="2"/>
+      <c r="BI9" s="2"/>
+      <c r="BJ9" s="2"/>
+      <c r="BK9" s="2"/>
     </row>
-    <row r="10" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
+    <row r="10" spans="1:63" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="4"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="7"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
       <c r="M10" s="3"/>
       <c r="N10" s="3"/>
       <c r="O10" s="3"/>
-      <c r="P10" s="8"/>
-      <c r="Q10" s="7"/>
-      <c r="R10" s="8"/>
-      <c r="S10" s="7"/>
-      <c r="T10" s="7"/>
-      <c r="U10" s="7"/>
+      <c r="P10" s="5"/>
+      <c r="Q10" s="4"/>
+      <c r="R10" s="5"/>
+      <c r="S10" s="4"/>
+      <c r="T10" s="4"/>
+      <c r="U10" s="4"/>
       <c r="V10" s="3"/>
       <c r="W10" s="3"/>
       <c r="X10" s="3"/>
       <c r="Y10" s="3"/>
       <c r="Z10" s="3"/>
       <c r="AA10" s="3"/>
-      <c r="AB10" s="9"/>
-      <c r="AC10" s="9"/>
-      <c r="AD10" s="9"/>
-      <c r="AE10" s="9"/>
+      <c r="AB10" s="6"/>
+      <c r="AC10" s="6"/>
+      <c r="AD10" s="6"/>
+      <c r="AE10" s="6"/>
       <c r="AF10" s="2"/>
       <c r="AG10" s="2"/>
       <c r="AH10" s="2"/>
@@ -1069,41 +1306,62 @@
       <c r="AN10" s="2"/>
       <c r="AO10" s="2"/>
       <c r="AP10" s="2"/>
+      <c r="AQ10" s="2"/>
+      <c r="AR10" s="2"/>
+      <c r="AS10" s="2"/>
+      <c r="AT10" s="2"/>
+      <c r="AU10" s="2"/>
+      <c r="AV10" s="2"/>
+      <c r="AW10" s="2"/>
+      <c r="AX10" s="2"/>
+      <c r="AY10" s="2"/>
+      <c r="AZ10" s="2"/>
+      <c r="BA10" s="2"/>
+      <c r="BB10" s="2"/>
+      <c r="BC10" s="2"/>
+      <c r="BD10" s="2"/>
+      <c r="BE10" s="2"/>
+      <c r="BF10" s="2"/>
+      <c r="BG10" s="2"/>
+      <c r="BH10" s="2"/>
+      <c r="BI10" s="2"/>
+      <c r="BJ10" s="2"/>
+      <c r="BK10" s="2"/>
     </row>
-    <row r="11" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+    <row r="11" spans="1:63" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="4"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="7"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
       <c r="L11" s="2"/>
       <c r="M11" s="3"/>
       <c r="N11" s="3"/>
       <c r="O11" s="3"/>
-      <c r="P11" s="8"/>
-      <c r="Q11" s="7"/>
-      <c r="R11" s="8"/>
-      <c r="S11" s="7"/>
-      <c r="T11" s="7"/>
-      <c r="U11" s="7"/>
+      <c r="P11" s="5"/>
+      <c r="Q11" s="4"/>
+      <c r="R11" s="5"/>
+      <c r="S11" s="4"/>
+      <c r="T11" s="4"/>
+      <c r="U11" s="4"/>
       <c r="V11" s="3"/>
       <c r="W11" s="3"/>
       <c r="X11" s="3"/>
       <c r="Y11" s="3"/>
       <c r="Z11" s="3"/>
       <c r="AA11" s="3"/>
-      <c r="AB11" s="9"/>
-      <c r="AC11" s="9"/>
-      <c r="AD11" s="9"/>
-      <c r="AE11" s="9"/>
+      <c r="AB11" s="6"/>
+      <c r="AC11" s="6"/>
+      <c r="AD11" s="6"/>
+      <c r="AE11" s="6"/>
       <c r="AF11" s="2"/>
       <c r="AG11" s="2"/>
       <c r="AH11" s="2"/>
@@ -1115,41 +1373,62 @@
       <c r="AN11" s="2"/>
       <c r="AO11" s="2"/>
       <c r="AP11" s="2"/>
+      <c r="AQ11" s="2"/>
+      <c r="AR11" s="2"/>
+      <c r="AS11" s="2"/>
+      <c r="AT11" s="2"/>
+      <c r="AU11" s="2"/>
+      <c r="AV11" s="2"/>
+      <c r="AW11" s="2"/>
+      <c r="AX11" s="2"/>
+      <c r="AY11" s="2"/>
+      <c r="AZ11" s="2"/>
+      <c r="BA11" s="2"/>
+      <c r="BB11" s="2"/>
+      <c r="BC11" s="2"/>
+      <c r="BD11" s="2"/>
+      <c r="BE11" s="2"/>
+      <c r="BF11" s="2"/>
+      <c r="BG11" s="2"/>
+      <c r="BH11" s="2"/>
+      <c r="BI11" s="2"/>
+      <c r="BJ11" s="2"/>
+      <c r="BK11" s="2"/>
     </row>
-    <row r="12" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
+    <row r="12" spans="1:63" x14ac:dyDescent="0.25">
+      <c r="A12" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="4"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
-      <c r="I12" s="7"/>
+      <c r="B12" s="10"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
       <c r="M12" s="3"/>
       <c r="N12" s="3"/>
       <c r="O12" s="3"/>
-      <c r="P12" s="8"/>
-      <c r="Q12" s="7"/>
-      <c r="R12" s="8"/>
-      <c r="S12" s="8"/>
-      <c r="T12" s="8"/>
-      <c r="U12" s="8"/>
+      <c r="P12" s="5"/>
+      <c r="Q12" s="4"/>
+      <c r="R12" s="5"/>
+      <c r="S12" s="5"/>
+      <c r="T12" s="5"/>
+      <c r="U12" s="5"/>
       <c r="V12" s="3"/>
       <c r="W12" s="3"/>
       <c r="X12" s="3"/>
       <c r="Y12" s="3"/>
       <c r="Z12" s="3"/>
       <c r="AA12" s="3"/>
-      <c r="AB12" s="9"/>
-      <c r="AC12" s="9"/>
-      <c r="AD12" s="9"/>
-      <c r="AE12" s="9"/>
+      <c r="AB12" s="6"/>
+      <c r="AC12" s="6"/>
+      <c r="AD12" s="6"/>
+      <c r="AE12" s="6"/>
       <c r="AF12" s="2"/>
       <c r="AG12" s="2"/>
       <c r="AH12" s="2"/>
@@ -1161,21 +1440,44 @@
       <c r="AN12" s="2"/>
       <c r="AO12" s="2"/>
       <c r="AP12" s="2"/>
+      <c r="AQ12" s="2"/>
+      <c r="AR12" s="2"/>
+      <c r="AS12" s="2"/>
+      <c r="AT12" s="2"/>
+      <c r="AU12" s="2"/>
+      <c r="AV12" s="2"/>
+      <c r="AW12" s="2"/>
+      <c r="AX12" s="2"/>
+      <c r="AY12" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AZ12" s="2"/>
+      <c r="BA12" s="2"/>
+      <c r="BB12" s="2"/>
+      <c r="BC12" s="2"/>
+      <c r="BD12" s="2"/>
+      <c r="BE12" s="2"/>
+      <c r="BF12" s="2"/>
+      <c r="BG12" s="2"/>
+      <c r="BH12" s="2"/>
+      <c r="BI12" s="2"/>
+      <c r="BJ12" s="2"/>
+      <c r="BK12" s="2"/>
     </row>
-    <row r="13" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
+    <row r="13" spans="1:63" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="4"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="8" t="s">
+      <c r="B13" s="10"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
-      <c r="I13" s="7"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
@@ -1184,12 +1486,12 @@
       <c r="O13" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="P13" s="8"/>
-      <c r="Q13" s="7"/>
-      <c r="R13" s="8"/>
-      <c r="S13" s="8"/>
-      <c r="T13" s="8"/>
-      <c r="U13" s="8" t="s">
+      <c r="P13" s="5"/>
+      <c r="Q13" s="4"/>
+      <c r="R13" s="5"/>
+      <c r="S13" s="5"/>
+      <c r="T13" s="5"/>
+      <c r="U13" s="5" t="s">
         <v>41</v>
       </c>
       <c r="V13" s="3"/>
@@ -1200,10 +1502,10 @@
       <c r="AA13" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="AB13" s="9"/>
-      <c r="AC13" s="9"/>
-      <c r="AD13" s="9"/>
-      <c r="AE13" s="9"/>
+      <c r="AB13" s="6"/>
+      <c r="AC13" s="6"/>
+      <c r="AD13" s="6"/>
+      <c r="AE13" s="6"/>
       <c r="AF13" s="2"/>
       <c r="AG13" s="2"/>
       <c r="AH13" s="2" t="s">
@@ -1217,21 +1519,44 @@
       <c r="AN13" s="2"/>
       <c r="AO13" s="2"/>
       <c r="AP13" s="2"/>
+      <c r="AQ13" s="2"/>
+      <c r="AR13" s="2"/>
+      <c r="AS13" s="2"/>
+      <c r="AT13" s="2"/>
+      <c r="AU13" s="2"/>
+      <c r="AV13" s="2"/>
+      <c r="AW13" s="2"/>
+      <c r="AX13" s="2"/>
+      <c r="AY13" s="2"/>
+      <c r="AZ13" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="BA13" s="2"/>
+      <c r="BB13" s="2"/>
+      <c r="BC13" s="2"/>
+      <c r="BD13" s="2"/>
+      <c r="BE13" s="2"/>
+      <c r="BF13" s="2"/>
+      <c r="BG13" s="2"/>
+      <c r="BH13" s="2"/>
+      <c r="BI13" s="2"/>
+      <c r="BJ13" s="2"/>
+      <c r="BK13" s="2"/>
     </row>
-    <row r="14" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
+    <row r="14" spans="1:63" x14ac:dyDescent="0.25">
+      <c r="A14" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="4"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="8" t="s">
+      <c r="B14" s="10"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="G14" s="7"/>
-      <c r="H14" s="7"/>
-      <c r="I14" s="7"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
       <c r="J14" s="2"/>
       <c r="K14" s="3" t="s">
         <v>30</v>
@@ -1240,14 +1565,14 @@
       <c r="M14" s="3"/>
       <c r="N14" s="3"/>
       <c r="O14" s="3"/>
-      <c r="P14" s="7"/>
-      <c r="Q14" s="8" t="s">
+      <c r="P14" s="4"/>
+      <c r="Q14" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="R14" s="8"/>
-      <c r="S14" s="8"/>
-      <c r="T14" s="8"/>
-      <c r="U14" s="8"/>
+      <c r="R14" s="5"/>
+      <c r="S14" s="5"/>
+      <c r="T14" s="5"/>
+      <c r="U14" s="5"/>
       <c r="V14" s="3"/>
       <c r="W14" s="3" t="s">
         <v>48</v>
@@ -1256,10 +1581,10 @@
       <c r="Y14" s="3"/>
       <c r="Z14" s="3"/>
       <c r="AA14" s="3"/>
-      <c r="AB14" s="9"/>
-      <c r="AC14" s="9"/>
-      <c r="AD14" s="9"/>
-      <c r="AE14" s="9"/>
+      <c r="AB14" s="6"/>
+      <c r="AC14" s="6"/>
+      <c r="AD14" s="6"/>
+      <c r="AE14" s="6"/>
       <c r="AF14" s="2"/>
       <c r="AG14" s="2" t="s">
         <v>53</v>
@@ -1273,41 +1598,64 @@
       <c r="AN14" s="2"/>
       <c r="AO14" s="2"/>
       <c r="AP14" s="2"/>
+      <c r="AQ14" s="2"/>
+      <c r="AR14" s="2"/>
+      <c r="AS14" s="2"/>
+      <c r="AT14" s="2"/>
+      <c r="AU14" s="2"/>
+      <c r="AV14" s="2"/>
+      <c r="AW14" s="2"/>
+      <c r="AX14" s="2"/>
+      <c r="AY14" s="2"/>
+      <c r="AZ14" s="2"/>
+      <c r="BA14" s="2"/>
+      <c r="BB14" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="BC14" s="2"/>
+      <c r="BD14" s="2"/>
+      <c r="BE14" s="2"/>
+      <c r="BF14" s="2"/>
+      <c r="BG14" s="2"/>
+      <c r="BH14" s="2"/>
+      <c r="BI14" s="2"/>
+      <c r="BJ14" s="2"/>
+      <c r="BK14" s="2"/>
     </row>
-    <row r="15" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
+    <row r="15" spans="1:63" x14ac:dyDescent="0.25">
+      <c r="A15" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="4"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="7"/>
-      <c r="I15" s="7"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
       <c r="L15" s="2"/>
       <c r="M15" s="3"/>
       <c r="N15" s="3"/>
       <c r="O15" s="3"/>
-      <c r="P15" s="8"/>
-      <c r="Q15" s="7"/>
-      <c r="R15" s="8"/>
-      <c r="S15" s="8"/>
-      <c r="T15" s="8"/>
-      <c r="U15" s="8"/>
+      <c r="P15" s="5"/>
+      <c r="Q15" s="4"/>
+      <c r="R15" s="5"/>
+      <c r="S15" s="5"/>
+      <c r="T15" s="5"/>
+      <c r="U15" s="5"/>
       <c r="V15" s="3"/>
       <c r="W15" s="3"/>
       <c r="X15" s="3"/>
       <c r="Y15" s="3"/>
       <c r="Z15" s="3"/>
       <c r="AA15" s="3"/>
-      <c r="AB15" s="9"/>
-      <c r="AC15" s="9"/>
-      <c r="AD15" s="9"/>
-      <c r="AE15" s="9"/>
+      <c r="AB15" s="6"/>
+      <c r="AC15" s="6"/>
+      <c r="AD15" s="6"/>
+      <c r="AE15" s="6"/>
       <c r="AF15" s="2"/>
       <c r="AG15" s="2"/>
       <c r="AH15" s="2"/>
@@ -1319,21 +1667,42 @@
       <c r="AN15" s="2"/>
       <c r="AO15" s="2"/>
       <c r="AP15" s="2"/>
+      <c r="AQ15" s="2"/>
+      <c r="AR15" s="2"/>
+      <c r="AS15" s="2"/>
+      <c r="AT15" s="2"/>
+      <c r="AU15" s="2"/>
+      <c r="AV15" s="2"/>
+      <c r="AW15" s="2"/>
+      <c r="AX15" s="2"/>
+      <c r="AY15" s="2"/>
+      <c r="AZ15" s="2"/>
+      <c r="BA15" s="2"/>
+      <c r="BB15" s="2"/>
+      <c r="BC15" s="2"/>
+      <c r="BD15" s="2"/>
+      <c r="BE15" s="2"/>
+      <c r="BF15" s="2"/>
+      <c r="BG15" s="2"/>
+      <c r="BH15" s="2"/>
+      <c r="BI15" s="2"/>
+      <c r="BJ15" s="2"/>
+      <c r="BK15" s="2"/>
     </row>
-    <row r="16" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
+    <row r="16" spans="1:63" x14ac:dyDescent="0.25">
+      <c r="A16" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="4"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="8" t="s">
+      <c r="B16" s="10"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="H16" s="7"/>
-      <c r="I16" s="7"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
       <c r="L16" s="2"/>
@@ -1342,14 +1711,14 @@
         <v>33</v>
       </c>
       <c r="O16" s="3"/>
-      <c r="P16" s="8"/>
-      <c r="Q16" s="7"/>
-      <c r="R16" s="8"/>
-      <c r="S16" s="8"/>
-      <c r="T16" s="8" t="s">
+      <c r="P16" s="5"/>
+      <c r="Q16" s="4"/>
+      <c r="R16" s="5"/>
+      <c r="S16" s="5"/>
+      <c r="T16" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="U16" s="8"/>
+      <c r="U16" s="5"/>
       <c r="V16" s="3"/>
       <c r="W16" s="3"/>
       <c r="X16" s="3"/>
@@ -1358,10 +1727,10 @@
         <v>46</v>
       </c>
       <c r="AA16" s="3"/>
-      <c r="AB16" s="9"/>
-      <c r="AC16" s="9"/>
-      <c r="AD16" s="9"/>
-      <c r="AE16" s="9"/>
+      <c r="AB16" s="6"/>
+      <c r="AC16" s="6"/>
+      <c r="AD16" s="6"/>
+      <c r="AE16" s="6"/>
       <c r="AF16" s="2"/>
       <c r="AG16" s="2"/>
       <c r="AH16" s="2"/>
@@ -1375,21 +1744,44 @@
       <c r="AN16" s="2"/>
       <c r="AO16" s="2"/>
       <c r="AP16" s="2"/>
+      <c r="AQ16" s="2"/>
+      <c r="AR16" s="2"/>
+      <c r="AS16" s="2"/>
+      <c r="AT16" s="2"/>
+      <c r="AU16" s="2"/>
+      <c r="AV16" s="2"/>
+      <c r="AW16" s="2"/>
+      <c r="AX16" s="2"/>
+      <c r="AY16" s="2"/>
+      <c r="AZ16" s="2"/>
+      <c r="BA16" s="2"/>
+      <c r="BB16" s="2"/>
+      <c r="BC16" s="2"/>
+      <c r="BD16" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="BE16" s="2"/>
+      <c r="BF16" s="2"/>
+      <c r="BG16" s="2"/>
+      <c r="BH16" s="2"/>
+      <c r="BI16" s="2"/>
+      <c r="BJ16" s="2"/>
+      <c r="BK16" s="2"/>
     </row>
-    <row r="17" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
+    <row r="17" spans="1:63" x14ac:dyDescent="0.25">
+      <c r="A17" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="4"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="8" t="s">
+      <c r="B17" s="10"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="I17" s="7"/>
+      <c r="I17" s="4"/>
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
       <c r="L17" s="2"/>
@@ -1398,14 +1790,14 @@
       </c>
       <c r="N17" s="3"/>
       <c r="O17" s="3"/>
-      <c r="P17" s="8"/>
-      <c r="Q17" s="7"/>
-      <c r="R17" s="8"/>
-      <c r="S17" s="8" t="s">
+      <c r="P17" s="5"/>
+      <c r="Q17" s="4"/>
+      <c r="R17" s="5"/>
+      <c r="S17" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="T17" s="8"/>
-      <c r="U17" s="8"/>
+      <c r="T17" s="5"/>
+      <c r="U17" s="5"/>
       <c r="V17" s="3"/>
       <c r="W17" s="3"/>
       <c r="X17" s="3"/>
@@ -1414,10 +1806,10 @@
       </c>
       <c r="Z17" s="3"/>
       <c r="AA17" s="3"/>
-      <c r="AB17" s="9"/>
-      <c r="AC17" s="9"/>
-      <c r="AD17" s="9"/>
-      <c r="AE17" s="9"/>
+      <c r="AB17" s="6"/>
+      <c r="AC17" s="6"/>
+      <c r="AD17" s="6"/>
+      <c r="AE17" s="6"/>
       <c r="AF17" s="2"/>
       <c r="AG17" s="2"/>
       <c r="AH17" s="2"/>
@@ -1431,19 +1823,42 @@
       <c r="AN17" s="2"/>
       <c r="AO17" s="2"/>
       <c r="AP17" s="2"/>
+      <c r="AQ17" s="2"/>
+      <c r="AR17" s="2"/>
+      <c r="AS17" s="2"/>
+      <c r="AT17" s="2"/>
+      <c r="AU17" s="2"/>
+      <c r="AV17" s="2"/>
+      <c r="AW17" s="2"/>
+      <c r="AX17" s="2"/>
+      <c r="AY17" s="2"/>
+      <c r="AZ17" s="2"/>
+      <c r="BA17" s="2"/>
+      <c r="BB17" s="2"/>
+      <c r="BC17" s="2"/>
+      <c r="BD17" s="2"/>
+      <c r="BE17" s="2"/>
+      <c r="BF17" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="BG17" s="2"/>
+      <c r="BH17" s="2"/>
+      <c r="BI17" s="2"/>
+      <c r="BJ17" s="2"/>
+      <c r="BK17" s="2"/>
     </row>
-    <row r="18" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
+    <row r="18" spans="1:63" x14ac:dyDescent="0.25">
+      <c r="A18" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="4"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="7"/>
-      <c r="I18" s="8" t="s">
+      <c r="B18" s="10"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="5" t="s">
         <v>27</v>
       </c>
       <c r="J18" s="2"/>
@@ -1454,14 +1869,14 @@
       <c r="M18" s="3"/>
       <c r="N18" s="3"/>
       <c r="O18" s="3"/>
-      <c r="P18" s="8"/>
-      <c r="Q18" s="7"/>
-      <c r="R18" s="8" t="s">
+      <c r="P18" s="5"/>
+      <c r="Q18" s="4"/>
+      <c r="R18" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="S18" s="8"/>
-      <c r="T18" s="8"/>
-      <c r="U18" s="8"/>
+      <c r="S18" s="5"/>
+      <c r="T18" s="5"/>
+      <c r="U18" s="5"/>
       <c r="V18" s="3"/>
       <c r="W18" s="3"/>
       <c r="X18" s="3" t="s">
@@ -1470,12 +1885,12 @@
       <c r="Y18" s="3"/>
       <c r="Z18" s="3"/>
       <c r="AA18" s="3"/>
-      <c r="AB18" s="9"/>
-      <c r="AC18" s="9"/>
-      <c r="AD18" s="9" t="s">
+      <c r="AB18" s="6"/>
+      <c r="AC18" s="6"/>
+      <c r="AD18" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="AE18" s="9"/>
+      <c r="AE18" s="6"/>
       <c r="AF18" s="2"/>
       <c r="AG18" s="2"/>
       <c r="AH18" s="2"/>
@@ -1487,41 +1902,64 @@
       <c r="AN18" s="2"/>
       <c r="AO18" s="2"/>
       <c r="AP18" s="2"/>
+      <c r="AQ18" s="2"/>
+      <c r="AR18" s="2"/>
+      <c r="AS18" s="2"/>
+      <c r="AT18" s="2"/>
+      <c r="AU18" s="2"/>
+      <c r="AV18" s="2"/>
+      <c r="AW18" s="2"/>
+      <c r="AX18" s="2"/>
+      <c r="AY18" s="2"/>
+      <c r="AZ18" s="2"/>
+      <c r="BA18" s="2"/>
+      <c r="BB18" s="2"/>
+      <c r="BC18" s="2"/>
+      <c r="BD18" s="2"/>
+      <c r="BE18" s="2"/>
+      <c r="BF18" s="2"/>
+      <c r="BG18" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="BH18" s="2"/>
+      <c r="BI18" s="2"/>
+      <c r="BJ18" s="2"/>
+      <c r="BK18" s="2"/>
     </row>
-    <row r="19" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
+    <row r="19" spans="1:63" x14ac:dyDescent="0.25">
+      <c r="A19" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="4"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="7"/>
-      <c r="I19" s="7"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
       <c r="M19" s="2"/>
       <c r="N19" s="2"/>
       <c r="O19" s="2"/>
-      <c r="P19" s="7"/>
-      <c r="Q19" s="7"/>
-      <c r="R19" s="7"/>
-      <c r="S19" s="7"/>
-      <c r="T19" s="7"/>
-      <c r="U19" s="7"/>
+      <c r="P19" s="4"/>
+      <c r="Q19" s="4"/>
+      <c r="R19" s="4"/>
+      <c r="S19" s="4"/>
+      <c r="T19" s="4"/>
+      <c r="U19" s="4"/>
       <c r="V19" s="3"/>
       <c r="W19" s="3"/>
       <c r="X19" s="3"/>
       <c r="Y19" s="3"/>
       <c r="Z19" s="3"/>
       <c r="AA19" s="3"/>
-      <c r="AB19" s="9"/>
-      <c r="AC19" s="9"/>
-      <c r="AD19" s="9"/>
-      <c r="AE19" s="9"/>
+      <c r="AB19" s="6"/>
+      <c r="AC19" s="6"/>
+      <c r="AD19" s="6"/>
+      <c r="AE19" s="6"/>
       <c r="AF19" s="2"/>
       <c r="AG19" s="2"/>
       <c r="AH19" s="2"/>
@@ -1535,41 +1973,64 @@
       <c r="AN19" s="2"/>
       <c r="AO19" s="2"/>
       <c r="AP19" s="2"/>
+      <c r="AQ19" s="2"/>
+      <c r="AR19" s="2"/>
+      <c r="AS19" s="2"/>
+      <c r="AT19" s="2"/>
+      <c r="AU19" s="2"/>
+      <c r="AV19" s="2"/>
+      <c r="AW19" s="2"/>
+      <c r="AX19" s="2"/>
+      <c r="AY19" s="2"/>
+      <c r="AZ19" s="2"/>
+      <c r="BA19" s="2"/>
+      <c r="BB19" s="2"/>
+      <c r="BC19" s="2"/>
+      <c r="BD19" s="2"/>
+      <c r="BE19" s="2"/>
+      <c r="BF19" s="2"/>
+      <c r="BG19" s="2"/>
+      <c r="BH19" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="BI19" s="2"/>
+      <c r="BJ19" s="2"/>
+      <c r="BK19" s="2"/>
     </row>
-    <row r="20" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
+    <row r="20" spans="1:63" x14ac:dyDescent="0.25">
+      <c r="A20" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="4"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="7"/>
-      <c r="I20" s="7"/>
+      <c r="B20" s="10"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="4"/>
       <c r="J20" s="2"/>
       <c r="K20" s="2"/>
       <c r="L20" s="2"/>
       <c r="M20" s="2"/>
       <c r="N20" s="2"/>
       <c r="O20" s="2"/>
-      <c r="P20" s="7"/>
-      <c r="Q20" s="7"/>
-      <c r="R20" s="7"/>
-      <c r="S20" s="7"/>
-      <c r="T20" s="7"/>
-      <c r="U20" s="7"/>
+      <c r="P20" s="4"/>
+      <c r="Q20" s="4"/>
+      <c r="R20" s="4"/>
+      <c r="S20" s="4"/>
+      <c r="T20" s="4"/>
+      <c r="U20" s="4"/>
       <c r="V20" s="2"/>
       <c r="W20" s="2"/>
       <c r="X20" s="2"/>
       <c r="Y20" s="2"/>
       <c r="Z20" s="2"/>
       <c r="AA20" s="2"/>
-      <c r="AB20" s="7"/>
-      <c r="AC20" s="7"/>
-      <c r="AD20" s="7"/>
-      <c r="AE20" s="7"/>
+      <c r="AB20" s="4"/>
+      <c r="AC20" s="4"/>
+      <c r="AD20" s="4"/>
+      <c r="AE20" s="4"/>
       <c r="AF20" s="2"/>
       <c r="AG20" s="2"/>
       <c r="AH20" s="2"/>
@@ -1581,41 +2042,64 @@
       <c r="AN20" s="2"/>
       <c r="AO20" s="2"/>
       <c r="AP20" s="2"/>
+      <c r="AQ20" s="2"/>
+      <c r="AR20" s="2"/>
+      <c r="AS20" s="2"/>
+      <c r="AT20" s="2"/>
+      <c r="AU20" s="2"/>
+      <c r="AV20" s="2"/>
+      <c r="AW20" s="2"/>
+      <c r="AX20" s="2"/>
+      <c r="AY20" s="2"/>
+      <c r="AZ20" s="2"/>
+      <c r="BA20" s="2"/>
+      <c r="BB20" s="2"/>
+      <c r="BC20" s="2"/>
+      <c r="BD20" s="2"/>
+      <c r="BE20" s="2"/>
+      <c r="BF20" s="2"/>
+      <c r="BG20" s="2"/>
+      <c r="BH20" s="2"/>
+      <c r="BI20" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="BJ20" s="2"/>
+      <c r="BK20" s="2"/>
     </row>
-    <row r="21" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
+    <row r="21" spans="1:63" x14ac:dyDescent="0.25">
+      <c r="A21" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="4"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="7"/>
-      <c r="H21" s="7"/>
-      <c r="I21" s="7"/>
+      <c r="B21" s="10"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
+      <c r="I21" s="4"/>
       <c r="J21" s="2"/>
       <c r="K21" s="2"/>
       <c r="L21" s="2"/>
       <c r="M21" s="2"/>
       <c r="N21" s="2"/>
       <c r="O21" s="2"/>
-      <c r="P21" s="7"/>
-      <c r="Q21" s="7"/>
-      <c r="R21" s="7"/>
-      <c r="S21" s="7"/>
-      <c r="T21" s="7"/>
-      <c r="U21" s="7"/>
+      <c r="P21" s="4"/>
+      <c r="Q21" s="4"/>
+      <c r="R21" s="4"/>
+      <c r="S21" s="4"/>
+      <c r="T21" s="4"/>
+      <c r="U21" s="4"/>
       <c r="V21" s="2"/>
       <c r="W21" s="2"/>
       <c r="X21" s="2"/>
       <c r="Y21" s="2"/>
       <c r="Z21" s="2"/>
       <c r="AA21" s="2"/>
-      <c r="AB21" s="7"/>
-      <c r="AC21" s="7"/>
-      <c r="AD21" s="7"/>
-      <c r="AE21" s="7"/>
+      <c r="AB21" s="4"/>
+      <c r="AC21" s="4"/>
+      <c r="AD21" s="4"/>
+      <c r="AE21" s="4"/>
       <c r="AF21" s="2"/>
       <c r="AG21" s="2"/>
       <c r="AH21" s="2"/>
@@ -1629,14 +2113,38 @@
       <c r="AN21" s="2"/>
       <c r="AO21" s="2"/>
       <c r="AP21" s="2"/>
+      <c r="AQ21" s="2"/>
+      <c r="AR21" s="2"/>
+      <c r="AS21" s="2"/>
+      <c r="AT21" s="2"/>
+      <c r="AU21" s="2"/>
+      <c r="AV21" s="2"/>
+      <c r="AW21" s="2"/>
+      <c r="AX21" s="2"/>
+      <c r="AY21" s="2"/>
+      <c r="AZ21" s="2"/>
+      <c r="BA21" s="2"/>
+      <c r="BB21" s="2"/>
+      <c r="BC21" s="2"/>
+      <c r="BD21" s="2"/>
+      <c r="BE21" s="2"/>
+      <c r="BF21" s="2"/>
+      <c r="BG21" s="2"/>
+      <c r="BH21" s="2"/>
+      <c r="BI21" s="2"/>
+      <c r="BJ21" s="2"/>
+      <c r="BK21" s="2" t="s">
+        <v>67</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="26">
-    <mergeCell ref="AB2:AE2"/>
-    <mergeCell ref="AF2:AP2"/>
-    <mergeCell ref="J2:O2"/>
-    <mergeCell ref="P2:U2"/>
-    <mergeCell ref="V2:AA2"/>
+  <mergeCells count="27">
+    <mergeCell ref="AQ2:BK2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A21:B21"/>
     <mergeCell ref="C2:I2"/>
@@ -1653,11 +2161,11 @@
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="AB2:AE2"/>
+    <mergeCell ref="AF2:AP2"/>
+    <mergeCell ref="J2:O2"/>
+    <mergeCell ref="P2:U2"/>
+    <mergeCell ref="V2:AA2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>